<commit_message>
Week 3 data plus conference stuff
</commit_message>
<xml_diff>
--- a/Cortisol Material/CortisolTimes.xlsx
+++ b/Cortisol Material/CortisolTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfv563\Git\Dissertation\Cortisol Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEFD91A-859D-4AA5-A65F-3281A6AA6C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F157A625-A491-4C6C-BDF4-DBE587174C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2438E2BD-FE6D-4608-AA45-6070093F68C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="28">
   <si>
     <t>Participant</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>participant forgot to do the cortisol collection the day after the cognitive task, so she collected it 2 days after instead (final time is technically the next day)</t>
+  </si>
+  <si>
+    <t>(final 2 times are technically the next day, and only 10 minutes apart)</t>
+  </si>
+  <si>
+    <t>(final 2 times are technically the next day, and only 15 minutes apart)</t>
   </si>
 </sst>
 </file>
@@ -470,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9244A2B-308D-47A2-B20C-98D7CFD4BB37}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,6 +566,21 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
+      <c r="C4" s="2">
+        <v>0.29930555555555555</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.98958333333333337</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -616,6 +637,24 @@
       </c>
       <c r="B7" s="1">
         <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.46250000000000002</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.83402777777777781</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -677,6 +716,24 @@
       <c r="B10" s="1">
         <v>3</v>
       </c>
+      <c r="C10" s="2">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -848,6 +905,21 @@
       <c r="B19" s="1">
         <v>3</v>
       </c>
+      <c r="C19" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.95833333333333337</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -908,6 +980,24 @@
       <c r="B22" s="1">
         <v>3</v>
       </c>
+      <c r="C22" s="2">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3.1944444444444442E-2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -971,7 +1061,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="H26" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1101,6 +1191,24 @@
       <c r="B33" s="1">
         <v>2</v>
       </c>
+      <c r="C33" s="2">
+        <v>0.2326388888888889</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="G33" s="2">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="H33" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -1143,6 +1251,24 @@
       <c r="B36" s="1">
         <v>2</v>
       </c>
+      <c r="C36" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="H36" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -1185,6 +1311,24 @@
       <c r="B39" s="1">
         <v>2</v>
       </c>
+      <c r="C39" s="2">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.70763888888888893</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.83680555555555558</v>
+      </c>
+      <c r="G39" s="2">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H39" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -1227,6 +1371,24 @@
       <c r="B42" s="1">
         <v>2</v>
       </c>
+      <c r="C42" s="2">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="G42" s="2">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="H42" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -1268,6 +1430,21 @@
       </c>
       <c r="B45" s="1">
         <v>2</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.32847222222222222</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0.68055555555555558</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
cortisol and schedule update
</commit_message>
<xml_diff>
--- a/Cortisol Material/CortisolTimes.xlsx
+++ b/Cortisol Material/CortisolTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfv563\Git\Dissertation\Cortisol Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F157A625-A491-4C6C-BDF4-DBE587174C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE45782-6B9D-4DC4-9839-07927C19CF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2438E2BD-FE6D-4608-AA45-6070093F68C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2438E2BD-FE6D-4608-AA45-6070093F68C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>Participant</t>
   </si>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9244A2B-308D-47A2-B20C-98D7CFD4BB37}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1217,6 +1217,24 @@
       <c r="B34" s="1">
         <v>3</v>
       </c>
+      <c r="C34" s="2">
+        <v>0.2388888888888889</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.27013888888888887</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.57222222222222219</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.73888888888888893</v>
+      </c>
+      <c r="G34" s="2">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">

</xml_diff>

<commit_message>
week 3 data updated
</commit_message>
<xml_diff>
--- a/Cortisol Material/CortisolTimes.xlsx
+++ b/Cortisol Material/CortisolTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfv563\Git\Dissertation\Cortisol Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F90EC2D-0992-4704-B800-8D7E115422AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE798A1-AB6B-4FEE-9875-90614361922C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2438E2BD-FE6D-4608-AA45-6070093F68C4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2438E2BD-FE6D-4608-AA45-6070093F68C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
   <si>
     <t>Participant</t>
   </si>
@@ -111,13 +111,13 @@
     <t>(final 2 times are technically the next day)</t>
   </si>
   <si>
-    <t>participant forgot to do the cortisol collection the day after the cognitive task, so she collected it 2 days after instead (final time is technically the next day)</t>
-  </si>
-  <si>
     <t>(final 2 times are technically the next day, and only 10 minutes apart)</t>
   </si>
   <si>
     <t>(final 2 times are technically the next day, and only 15 minutes apart)</t>
+  </si>
+  <si>
+    <t>participant forgot to do the cortisol collection the day after the cognitive task, so she collected it 2 days after the cog task instead (final time is technically the next day)</t>
   </si>
 </sst>
 </file>
@@ -476,15 +476,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9244A2B-308D-47A2-B20C-98D7CFD4BB37}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E24" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="134.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="145.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -654,7 +654,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -851,6 +851,24 @@
       <c r="B16" s="1">
         <v>3</v>
       </c>
+      <c r="C16" s="2">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.47152777777777777</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.69027777777777777</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.94027777777777777</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -1029,6 +1047,21 @@
       <c r="B24" s="1">
         <v>2</v>
       </c>
+      <c r="C24" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.36527777777777776</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.67152777777777772</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.97916666666666663</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -1061,7 +1094,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="H26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1087,7 +1120,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="H27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1312,6 +1345,24 @@
       </c>
       <c r="B37" s="1">
         <v>3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="G37" s="2">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="H37" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>